<commit_message>
Adding data driven approach from excel
</commit_message>
<xml_diff>
--- a/okCredit/src/resources/TestData.xlsx
+++ b/okCredit/src/resources/TestData.xlsx
@@ -11,37 +11,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>TestCase Name</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Source Currency</t>
-  </si>
-  <si>
-    <t>Destination Currency</t>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Customer Ph</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Payment</t>
   </si>
   <si>
     <t>TC_01</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>GBP</t>
+    <t>English</t>
+  </si>
+  <si>
+    <t>7406764431</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Test User 1</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Test User 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -62,6 +89,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -102,6 +130,10 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -331,10 +363,18 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -356,21 +396,27 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -390,6 +436,48 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>